<commit_message>
liquid sg article Tb correlation added
</commit_message>
<xml_diff>
--- a/content/downloads/notebooks/pretty_tables.xlsx
+++ b/content/downloads/notebooks/pretty_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricKim\Documents\aegis4048.github.io-source\content\downloads\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFD2BA7-66B2-4E45-B4E0-A959CAEB276D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7206096-3097-422E-BE2C-2F9DD0786FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="SCN" sheetId="3" r:id="rId3"/>
     <sheet name="SCN2" sheetId="4" r:id="rId4"/>
     <sheet name="SCN3" sheetId="5" r:id="rId5"/>
+    <sheet name="SCN3 V2" sheetId="7" r:id="rId6"/>
+    <sheet name="SCN Parameters" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="50">
   <si>
     <t>Slope</t>
   </si>
@@ -159,23 +161,112 @@
     <t>Extracted with thermo</t>
   </si>
   <si>
-    <t>SG [Eq-4]</t>
+    <t>θ</t>
   </si>
   <si>
-    <t>Tb [R] [Eq-1]</t>
+    <t>a2</t>
   </si>
   <si>
-    <t>New Model</t>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>Eq-1b (MW &lt; 136)</t>
+  </si>
+  <si>
+    <t>Coefs Fitted From:</t>
+  </si>
+  <si>
+    <t>Riazi &amp; Al-Shahhaf (1996)</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>For low BTEX gas</t>
+  </si>
+  <si>
+    <t>For high BTEX gas, or crude oil</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Eq-1a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (MW ≥ 136)</t>
+    </r>
+  </si>
+  <si>
+    <t>-1.718e-4</t>
+  </si>
+  <si>
+    <t>2.322e-2</t>
+  </si>
+  <si>
+    <t>-3.162e-1</t>
+  </si>
+  <si>
+    <t>3.018e-7</t>
+  </si>
+  <si>
+    <t>1.719e-2</t>
+  </si>
+  <si>
+    <t>-6.947e-2</t>
+  </si>
+  <si>
+    <t>4.439e-7</t>
+  </si>
+  <si>
+    <t>Original Data</t>
+  </si>
+  <si>
+    <t>Model Prediction</t>
+  </si>
+  <si>
+    <t>SG [Eq-1]</t>
+  </si>
+  <si>
+    <t>Tb [R] [Eq-A]</t>
+  </si>
+  <si>
+    <t>Katz &amp; Al-Firoozabadi (1978)</t>
+  </si>
+  <si>
+    <t>SG [Eq-1b]</t>
+  </si>
+  <si>
+    <t>Training data source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -218,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +343,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -705,6 +802,89 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -720,38 +900,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,15 +1076,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>306457</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>226944</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -871,8 +1100,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14392275" y="4352925"/>
-          <a:ext cx="5410200" cy="3800475"/>
+          <a:off x="15529892" y="3341204"/>
+          <a:ext cx="5436704" cy="3800475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1008,6 +1237,81 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Tbs = np.array([ureg('%.15f kelvin' % Tb).to('rankine')._magnitude for Tb in Tbs])</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755430</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>387567</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>78828</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B1A95D8-71A6-E1E0-42D3-E404AB0B7E1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1845878" y="4243552"/>
+          <a:ext cx="2200603" cy="433552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:alpha val="17000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>aegis4048.github.io</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1531,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77638572-6EE6-4869-9ED2-03E08A7DFBD6}">
   <dimension ref="B1:X49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K49"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X36" sqref="B36:X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1855,9 @@
     <col min="14" max="14" width="9.140625" style="28"/>
     <col min="15" max="17" width="9.140625" style="23"/>
     <col min="18" max="18" width="9.140625" style="25"/>
-    <col min="19" max="16384" width="9.140625" style="23"/>
+    <col min="19" max="23" width="9.140625" style="23"/>
+    <col min="24" max="24" width="10.5703125" style="89" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
@@ -1562,26 +1868,26 @@
     <row r="2" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:24" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="61" t="s">
+      <c r="D3" s="91"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64" t="s">
+      <c r="G3" s="91"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="64"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="61" t="s">
+      <c r="J3" s="93"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="62"/>
-      <c r="N3" s="63"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="92"/>
       <c r="Q3" s="23" t="s">
         <v>19</v>
       </c>
@@ -1650,7 +1956,7 @@
       <c r="W4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="X4" s="23" t="s">
+      <c r="X4" s="89" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1717,7 +2023,7 @@
       <c r="W5" s="25">
         <v>0.68500000000000005</v>
       </c>
-      <c r="X5" s="23">
+      <c r="X5" s="89">
         <v>147</v>
       </c>
     </row>
@@ -1784,7 +2090,7 @@
       <c r="W6" s="25">
         <v>0.72199999999999998</v>
       </c>
-      <c r="X6" s="23">
+      <c r="X6" s="89">
         <v>197.5</v>
       </c>
     </row>
@@ -1851,7 +2157,7 @@
       <c r="W7" s="25">
         <v>0.745</v>
       </c>
-      <c r="X7" s="23">
+      <c r="X7" s="89">
         <v>242</v>
       </c>
     </row>
@@ -1918,7 +2224,7 @@
       <c r="W8" s="25">
         <v>0.76400000000000001</v>
       </c>
-      <c r="X8" s="23">
+      <c r="X8" s="89">
         <v>288</v>
       </c>
     </row>
@@ -1985,7 +2291,7 @@
       <c r="W9" s="25">
         <v>0.77800000000000002</v>
       </c>
-      <c r="X9" s="23">
+      <c r="X9" s="89">
         <v>330.5</v>
       </c>
     </row>
@@ -2052,7 +2358,7 @@
       <c r="W10" s="25">
         <v>0.78900000000000003</v>
       </c>
-      <c r="X10" s="23">
+      <c r="X10" s="89">
         <v>369</v>
       </c>
     </row>
@@ -2119,7 +2425,7 @@
       <c r="W11" s="25">
         <v>0.8</v>
       </c>
-      <c r="X11" s="23">
+      <c r="X11" s="89">
         <v>407</v>
       </c>
     </row>
@@ -2186,7 +2492,7 @@
       <c r="W12" s="25">
         <v>0.81100000000000005</v>
       </c>
-      <c r="X12" s="23">
+      <c r="X12" s="89">
         <v>441</v>
       </c>
     </row>
@@ -2253,7 +2559,7 @@
       <c r="W13" s="25">
         <v>0.82199999999999995</v>
       </c>
-      <c r="X13" s="23">
+      <c r="X13" s="89">
         <v>475.5</v>
       </c>
     </row>
@@ -2320,7 +2626,7 @@
       <c r="W14" s="25">
         <v>0.83199999999999996</v>
       </c>
-      <c r="X14" s="23">
+      <c r="X14" s="89">
         <v>511</v>
       </c>
     </row>
@@ -2387,7 +2693,7 @@
       <c r="W15" s="25">
         <v>0.83899999999999997</v>
       </c>
-      <c r="X15" s="23">
+      <c r="X15" s="89">
         <v>542</v>
       </c>
     </row>
@@ -2452,7 +2758,7 @@
       <c r="W16" s="25">
         <v>0.84699999999999998</v>
       </c>
-      <c r="X16" s="23">
+      <c r="X16" s="89">
         <v>572</v>
       </c>
     </row>
@@ -2517,7 +2823,7 @@
       <c r="W17" s="25">
         <v>0.85199999999999998</v>
       </c>
-      <c r="X17" s="23">
+      <c r="X17" s="89">
         <v>595</v>
       </c>
     </row>
@@ -2582,7 +2888,7 @@
       <c r="W18" s="25">
         <v>0.85699999999999998</v>
       </c>
-      <c r="X18" s="23">
+      <c r="X18" s="89">
         <v>617</v>
       </c>
     </row>
@@ -2647,7 +2953,7 @@
       <c r="W19" s="25">
         <v>0.86199999999999999</v>
       </c>
-      <c r="X19" s="23">
+      <c r="X19" s="89">
         <v>640.5</v>
       </c>
     </row>
@@ -2712,7 +3018,7 @@
       <c r="W20" s="25">
         <v>0.86699999999999999</v>
       </c>
-      <c r="X20" s="23">
+      <c r="X20" s="89">
         <v>664</v>
       </c>
     </row>
@@ -2777,7 +3083,7 @@
       <c r="W21" s="25">
         <v>0.872</v>
       </c>
-      <c r="X21" s="23">
+      <c r="X21" s="89">
         <v>686</v>
       </c>
     </row>
@@ -2842,7 +3148,7 @@
       <c r="W22" s="25">
         <v>0.877</v>
       </c>
-      <c r="X22" s="23">
+      <c r="X22" s="89">
         <v>707</v>
       </c>
     </row>
@@ -2907,7 +3213,7 @@
       <c r="W23" s="25">
         <v>0.88100000000000001</v>
       </c>
-      <c r="X23" s="23">
+      <c r="X23" s="89">
         <v>727</v>
       </c>
     </row>
@@ -2972,7 +3278,7 @@
       <c r="W24" s="25">
         <v>0.88500000000000001</v>
       </c>
-      <c r="X24" s="23">
+      <c r="X24" s="89">
         <v>747</v>
       </c>
     </row>
@@ -3037,7 +3343,7 @@
       <c r="W25" s="25">
         <v>0.88900000000000001</v>
       </c>
-      <c r="X25" s="23">
+      <c r="X25" s="89">
         <v>766</v>
       </c>
     </row>
@@ -3102,7 +3408,7 @@
       <c r="W26" s="25">
         <v>0.89300000000000002</v>
       </c>
-      <c r="X26" s="23">
+      <c r="X26" s="89">
         <v>784</v>
       </c>
     </row>
@@ -3167,7 +3473,7 @@
       <c r="W27" s="25">
         <v>0.89600000000000002</v>
       </c>
-      <c r="X27" s="23">
+      <c r="X27" s="89">
         <v>802</v>
       </c>
     </row>
@@ -3232,7 +3538,7 @@
       <c r="W28" s="25">
         <v>0.89900000000000002</v>
       </c>
-      <c r="X28" s="23">
+      <c r="X28" s="89">
         <v>817</v>
       </c>
     </row>
@@ -3297,7 +3603,7 @@
       <c r="W29" s="25">
         <v>0.90200000000000002</v>
       </c>
-      <c r="X29" s="23">
+      <c r="X29" s="89">
         <v>834</v>
       </c>
     </row>
@@ -3362,7 +3668,7 @@
       <c r="W30" s="25">
         <v>0.90600000000000003</v>
       </c>
-      <c r="X30" s="23">
+      <c r="X30" s="89">
         <v>850</v>
       </c>
     </row>
@@ -3427,7 +3733,7 @@
       <c r="W31" s="25">
         <v>0.90900000000000003</v>
       </c>
-      <c r="X31" s="23">
+      <c r="X31" s="89">
         <v>866</v>
       </c>
     </row>
@@ -3492,7 +3798,7 @@
       <c r="W32" s="25">
         <v>0.91200000000000003</v>
       </c>
-      <c r="X32" s="23">
+      <c r="X32" s="89">
         <v>881</v>
       </c>
     </row>
@@ -3557,7 +3863,7 @@
       <c r="W33" s="25">
         <v>0.91400000000000003</v>
       </c>
-      <c r="X33" s="23">
+      <c r="X33" s="89">
         <v>895</v>
       </c>
     </row>
@@ -3622,7 +3928,7 @@
       <c r="W34" s="25">
         <v>0.91700000000000004</v>
       </c>
-      <c r="X34" s="23">
+      <c r="X34" s="89">
         <v>908</v>
       </c>
     </row>
@@ -3687,7 +3993,7 @@
       <c r="W35" s="25">
         <v>0.91900000000000004</v>
       </c>
-      <c r="X35" s="23">
+      <c r="X35" s="89">
         <v>922</v>
       </c>
     </row>
@@ -3703,7 +4009,7 @@
       </c>
       <c r="E36" s="26">
         <f t="shared" si="0"/>
-        <v>1293.67</v>
+        <v>1393.67</v>
       </c>
       <c r="F36" s="24">
         <v>464</v>
@@ -3752,8 +4058,8 @@
       <c r="W36" s="25">
         <v>0.92200000000000004</v>
       </c>
-      <c r="X36" s="23">
-        <v>834</v>
+      <c r="X36" s="89">
+        <v>934</v>
       </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
@@ -3817,7 +4123,7 @@
       <c r="W37" s="25">
         <v>0.92400000000000004</v>
       </c>
-      <c r="X37" s="23">
+      <c r="X37" s="89">
         <v>947</v>
       </c>
     </row>
@@ -3882,7 +4188,7 @@
       <c r="W38" s="25">
         <v>0.92600000000000005</v>
       </c>
-      <c r="X38" s="23">
+      <c r="X38" s="89">
         <v>959</v>
       </c>
     </row>
@@ -3947,7 +4253,7 @@
       <c r="W39" s="25">
         <v>0.92800000000000005</v>
       </c>
-      <c r="X39" s="23">
+      <c r="X39" s="89">
         <v>972</v>
       </c>
     </row>
@@ -4012,7 +4318,7 @@
       <c r="W40" s="25">
         <v>0.93</v>
       </c>
-      <c r="X40" s="23">
+      <c r="X40" s="89">
         <v>982</v>
       </c>
     </row>
@@ -4077,7 +4383,7 @@
       <c r="W41" s="25">
         <v>0.93100000000000005</v>
       </c>
-      <c r="X41" s="23">
+      <c r="X41" s="89">
         <v>993</v>
       </c>
     </row>
@@ -4142,7 +4448,7 @@
       <c r="W42" s="25">
         <v>0.93300000000000005</v>
       </c>
-      <c r="X42" s="23">
+      <c r="X42" s="89">
         <v>1004</v>
       </c>
     </row>
@@ -4207,7 +4513,7 @@
       <c r="W43" s="25">
         <v>0.93500000000000005</v>
       </c>
-      <c r="X43" s="23">
+      <c r="X43" s="89">
         <v>1017</v>
       </c>
     </row>
@@ -4272,7 +4578,7 @@
       <c r="W44" s="25">
         <v>0.93700000000000006</v>
       </c>
-      <c r="X44" s="23">
+      <c r="X44" s="89">
         <v>1027</v>
       </c>
     </row>
@@ -4503,8 +4809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A0E854-CF57-42A5-A77F-FFC7ED373A0F}">
   <dimension ref="B1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4529,21 +4835,21 @@
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53"/>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="64" t="s">
+      <c r="D3" s="91"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="64"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="61" t="s">
+      <c r="G3" s="93"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="62"/>
-      <c r="K3" s="63"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="92"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="54" t="s">
@@ -5540,7 +5846,7 @@
         <v>0.92200000000000004</v>
       </c>
       <c r="E36" s="26">
-        <v>1293.67</v>
+        <v>1393.67</v>
       </c>
       <c r="F36" s="23">
         <v>513</v>
@@ -5929,10 +6235,1488 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C7F716-4E28-4058-88C8-028B61C51997}">
-  <dimension ref="B2:L33"/>
+  <dimension ref="B1:L60"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="103"/>
+    <col min="2" max="2" width="7.140625" style="100" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="101" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="100" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="101" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="102" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="103" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="103" customWidth="1"/>
+    <col min="9" max="9" width="12" style="103" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="104" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="103" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="103" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="103"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="107"/>
+      <c r="I2" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="107"/>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="63"/>
+      <c r="C3" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="92"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="92"/>
+      <c r="K3" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="92"/>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="108">
+        <v>80</v>
+      </c>
+      <c r="C5" s="109">
+        <v>0.6691568</v>
+      </c>
+      <c r="D5" s="110">
+        <v>599.43028279058797</v>
+      </c>
+      <c r="E5" s="111">
+        <v>0.6832916</v>
+      </c>
+      <c r="F5" s="110">
+        <v>599.923414370513</v>
+      </c>
+      <c r="H5" s="112">
+        <v>108</v>
+      </c>
+      <c r="I5" s="109">
+        <v>0.74687095680000004</v>
+      </c>
+      <c r="J5" s="110">
+        <v>599.923414370513</v>
+      </c>
+      <c r="K5" s="113">
+        <v>0.75122148160000002</v>
+      </c>
+      <c r="L5" s="114">
+        <v>704.22629768347099</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="115">
+        <v>81</v>
+      </c>
+      <c r="C6" s="116">
+        <v>0.67334685989999998</v>
+      </c>
+      <c r="D6" s="117">
+        <v>603.49917443890001</v>
+      </c>
+      <c r="E6" s="118">
+        <v>0.68680349380000005</v>
+      </c>
+      <c r="F6" s="117">
+        <v>603.99355603936101</v>
+      </c>
+      <c r="H6" s="115">
+        <v>109</v>
+      </c>
+      <c r="I6" s="116">
+        <v>0.74848757310000003</v>
+      </c>
+      <c r="J6" s="117">
+        <v>603.99355603936101</v>
+      </c>
+      <c r="K6" s="118">
+        <v>0.75272635219999995</v>
+      </c>
+      <c r="L6" s="117">
+        <v>707.625824946899</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="112">
+        <v>82</v>
+      </c>
+      <c r="C7" s="119">
+        <v>0.67740905520000005</v>
+      </c>
+      <c r="D7" s="114">
+        <v>607.539109294696</v>
+      </c>
+      <c r="E7" s="113">
+        <v>0.69021926239999998</v>
+      </c>
+      <c r="F7" s="114">
+        <v>608.03474608671502</v>
+      </c>
+      <c r="H7" s="112">
+        <v>110</v>
+      </c>
+      <c r="I7" s="119">
+        <v>0.75005089999999996</v>
+      </c>
+      <c r="J7" s="114">
+        <v>608.03474608671502</v>
+      </c>
+      <c r="K7" s="113">
+        <v>0.75418580000000002</v>
+      </c>
+      <c r="L7" s="114">
+        <v>711.00570380830504</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="115">
+        <v>83</v>
+      </c>
+      <c r="C8" s="116">
+        <v>0.68134604929999998</v>
+      </c>
+      <c r="D8" s="117">
+        <v>611.55054432043403</v>
+      </c>
+      <c r="E8" s="118">
+        <v>0.69354071660000005</v>
+      </c>
+      <c r="F8" s="117">
+        <v>612.04744135997601</v>
+      </c>
+      <c r="H8" s="115">
+        <v>111</v>
+      </c>
+      <c r="I8" s="116">
+        <v>0.75156360089999996</v>
+      </c>
+      <c r="J8" s="117">
+        <v>612.04744135997601</v>
+      </c>
+      <c r="K8" s="118">
+        <v>0.75560163579999995</v>
+      </c>
+      <c r="L8" s="117">
+        <v>714.36616922829205</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="112">
+        <v>84</v>
+      </c>
+      <c r="C9" s="119">
+        <v>0.68516050559999897</v>
+      </c>
+      <c r="D9" s="114">
+        <v>615.53392409052105</v>
+      </c>
+      <c r="E9" s="113">
+        <v>0.6967696672</v>
+      </c>
+      <c r="F9" s="114">
+        <v>616.03208632144595</v>
+      </c>
+      <c r="H9" s="112">
+        <v>112</v>
+      </c>
+      <c r="I9" s="119">
+        <v>0.75302833920000001</v>
+      </c>
+      <c r="J9" s="114">
+        <v>616.03208632144595</v>
+      </c>
+      <c r="K9" s="113">
+        <v>0.75697567040000002</v>
+      </c>
+      <c r="L9" s="114">
+        <v>717.70745141025998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="115">
+        <v>85</v>
+      </c>
+      <c r="C10" s="116">
+        <v>0.68885508749999902</v>
+      </c>
+      <c r="D10" s="117">
+        <v>619.48968127158696</v>
+      </c>
+      <c r="E10" s="118">
+        <v>0.69990792499999999</v>
+      </c>
+      <c r="F10" s="117">
+        <v>619.989113528487</v>
+      </c>
+      <c r="H10" s="115">
+        <v>113</v>
+      </c>
+      <c r="I10" s="116">
+        <v>0.75444777829999998</v>
+      </c>
+      <c r="J10" s="117">
+        <v>619.989113528487</v>
+      </c>
+      <c r="K10" s="118">
+        <v>0.75830971459999996</v>
+      </c>
+      <c r="L10" s="117">
+        <v>721.02977593836795</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="112">
+        <v>86</v>
+      </c>
+      <c r="C11" s="119">
+        <v>0.69243245840000001</v>
+      </c>
+      <c r="D11" s="114">
+        <v>623.41823707865001</v>
+      </c>
+      <c r="E11" s="113">
+        <v>0.70295730079999996</v>
+      </c>
+      <c r="F11" s="114">
+        <v>623.91894408959001</v>
+      </c>
+      <c r="H11" s="112">
+        <v>114</v>
+      </c>
+      <c r="I11" s="119">
+        <v>0.75582458159999999</v>
+      </c>
+      <c r="J11" s="114">
+        <v>623.91894408959001</v>
+      </c>
+      <c r="K11" s="113">
+        <v>0.75960557920000005</v>
+      </c>
+      <c r="L11" s="114">
+        <v>724.333363910304</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="115">
+        <v>87</v>
+      </c>
+      <c r="C12" s="116">
+        <v>0.69589528170000003</v>
+      </c>
+      <c r="D12" s="117">
+        <v>627.32000170866604</v>
+      </c>
+      <c r="E12" s="118">
+        <v>0.70591960539999998</v>
+      </c>
+      <c r="F12" s="117">
+        <v>627.82198809782597</v>
+      </c>
+      <c r="H12" s="115">
+        <v>115</v>
+      </c>
+      <c r="I12" s="116">
+        <v>0.75716141250000002</v>
+      </c>
+      <c r="J12" s="117">
+        <v>627.82198809782597</v>
+      </c>
+      <c r="K12" s="118">
+        <v>0.760865075</v>
+      </c>
+      <c r="L12" s="117">
+        <v>727.618432065094</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="112">
+        <v>88</v>
+      </c>
+      <c r="C13" s="119">
+        <v>0.69924622079999998</v>
+      </c>
+      <c r="D13" s="114">
+        <v>631.19537475282698</v>
+      </c>
+      <c r="E13" s="113">
+        <v>0.70879664959999999</v>
+      </c>
+      <c r="F13" s="114">
+        <v>631.69864504305497</v>
+      </c>
+      <c r="H13" s="112">
+        <v>116</v>
+      </c>
+      <c r="I13" s="119">
+        <v>0.75846093439999995</v>
+      </c>
+      <c r="J13" s="114">
+        <v>631.69864504305497</v>
+      </c>
+      <c r="K13" s="113">
+        <v>0.76209001279999999</v>
+      </c>
+      <c r="L13" s="114">
+        <v>730.88519290618603</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="115">
+        <v>89</v>
+      </c>
+      <c r="C14" s="116">
+        <v>0.70248793909999996</v>
+      </c>
+      <c r="D14" s="117">
+        <v>635.04474558887102</v>
+      </c>
+      <c r="E14" s="118">
+        <v>0.71159024420000005</v>
+      </c>
+      <c r="F14" s="117">
+        <v>635.54930420414905</v>
+      </c>
+      <c r="H14" s="115">
+        <v>117</v>
+      </c>
+      <c r="I14" s="116">
+        <v>0.7597258107</v>
+      </c>
+      <c r="J14" s="117">
+        <v>635.54930420414905</v>
+      </c>
+      <c r="K14" s="118">
+        <v>0.76328220339999997</v>
+      </c>
+      <c r="L14" s="117">
+        <v>734.13385482000797</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="112">
+        <v>90</v>
+      </c>
+      <c r="C15" s="119">
+        <v>0.70562309999999895</v>
+      </c>
+      <c r="D15" s="114">
+        <v>638.86849375461702</v>
+      </c>
+      <c r="E15" s="113">
+        <v>0.7143022</v>
+      </c>
+      <c r="F15" s="114">
+        <v>639.37434502243798</v>
+      </c>
+      <c r="H15" s="112">
+        <v>118</v>
+      </c>
+      <c r="I15" s="119">
+        <v>0.76095870480000005</v>
+      </c>
+      <c r="J15" s="114">
+        <v>639.37434502243798</v>
+      </c>
+      <c r="K15" s="113">
+        <v>0.76444345759999999</v>
+      </c>
+      <c r="L15" s="114">
+        <v>737.36462219023304</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="115">
+        <v>91</v>
+      </c>
+      <c r="C16" s="116">
+        <v>0.70865436690000005</v>
+      </c>
+      <c r="D16" s="117">
+        <v>642.66698930377902</v>
+      </c>
+      <c r="E16" s="118">
+        <v>0.71693432779999999</v>
+      </c>
+      <c r="F16" s="117">
+        <v>643.17413745745205</v>
+      </c>
+      <c r="H16" s="115">
+        <v>119</v>
+      </c>
+      <c r="I16" s="116">
+        <v>0.76216228009999998</v>
+      </c>
+      <c r="J16" s="117">
+        <v>643.17413745745205</v>
+      </c>
+      <c r="K16" s="118">
+        <v>0.76557558619999999</v>
+      </c>
+      <c r="L16" s="117">
+        <v>740.57769550789601</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="112">
+        <v>92</v>
+      </c>
+      <c r="C17" s="119">
+        <v>0.71158440319999905</v>
+      </c>
+      <c r="D17" s="114">
+        <v>646.44059314513299</v>
+      </c>
+      <c r="E17" s="113">
+        <v>0.71948843839999999</v>
+      </c>
+      <c r="F17" s="114">
+        <v>646.94904232600504</v>
+      </c>
+      <c r="H17" s="112">
+        <v>120</v>
+      </c>
+      <c r="I17" s="119">
+        <v>0.7633392</v>
+      </c>
+      <c r="J17" s="114">
+        <v>646.94904232600504</v>
+      </c>
+      <c r="K17" s="113">
+        <v>0.76668040000000004</v>
+      </c>
+      <c r="L17" s="114">
+        <v>743.77327147760195</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="115">
+        <v>93</v>
+      </c>
+      <c r="C18" s="116">
+        <v>0.71441587230000003</v>
+      </c>
+      <c r="D18" s="117">
+        <v>650.18965736595305</v>
+      </c>
+      <c r="E18" s="118">
+        <v>0.72196634260000003</v>
+      </c>
+      <c r="F18" s="117">
+        <v>650.69941162556097</v>
+      </c>
+      <c r="H18" s="115">
+        <v>121</v>
+      </c>
+      <c r="I18" s="116">
+        <v>0.76449212789999998</v>
+      </c>
+      <c r="J18" s="117">
+        <v>650.69941162556097</v>
+      </c>
+      <c r="K18" s="118">
+        <v>0.76775970979999997</v>
+      </c>
+      <c r="L18" s="117">
+        <v>746.95154311994702</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="112">
+        <v>94</v>
+      </c>
+      <c r="C19" s="119">
+        <v>0.717151437599999</v>
+      </c>
+      <c r="D19" s="114">
+        <v>653.91452554063005</v>
+      </c>
+      <c r="E19" s="113">
+        <v>0.72436985119999997</v>
+      </c>
+      <c r="F19" s="114">
+        <v>654.42558884278401</v>
+      </c>
+      <c r="H19" s="112">
+        <v>122</v>
+      </c>
+      <c r="I19" s="119">
+        <v>0.76562372720000005</v>
+      </c>
+      <c r="J19" s="114">
+        <v>654.42558884278401</v>
+      </c>
+      <c r="K19" s="113">
+        <v>0.76881532640000005</v>
+      </c>
+      <c r="L19" s="114">
+        <v>750.11269987034495</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="115">
+        <v>95</v>
+      </c>
+      <c r="C20" s="116">
+        <v>0.71979376250000005</v>
+      </c>
+      <c r="D20" s="117">
+        <v>657.61553302529296</v>
+      </c>
+      <c r="E20" s="118">
+        <v>0.72670077499999997</v>
+      </c>
+      <c r="F20" s="117">
+        <v>658.12790924809201</v>
+      </c>
+      <c r="H20" s="115">
+        <v>123</v>
+      </c>
+      <c r="I20" s="116">
+        <v>0.76673666129999996</v>
+      </c>
+      <c r="J20" s="117">
+        <v>658.12790924809201</v>
+      </c>
+      <c r="K20" s="118">
+        <v>0.76984906060000002</v>
+      </c>
+      <c r="L20" s="117">
+        <v>753.25692767441399</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="112">
+        <v>96</v>
+      </c>
+      <c r="C21" s="119">
+        <v>0.72234551039999995</v>
+      </c>
+      <c r="D21" s="114">
+        <v>661.29300723922097</v>
+      </c>
+      <c r="E21" s="113">
+        <v>0.72896092479999997</v>
+      </c>
+      <c r="F21" s="114">
+        <v>661.80670017700095</v>
+      </c>
+      <c r="H21" s="112">
+        <v>124</v>
+      </c>
+      <c r="I21" s="119">
+        <v>0.76783359360000003</v>
+      </c>
+      <c r="J21" s="114">
+        <v>661.80670017700095</v>
+      </c>
+      <c r="K21" s="113">
+        <v>0.77086272319999904</v>
+      </c>
+      <c r="L21" s="114">
+        <v>756.384409080056</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="115">
+        <v>97</v>
+      </c>
+      <c r="C22" s="116">
+        <v>0.72480934470000002</v>
+      </c>
+      <c r="D22" s="117">
+        <v>664.947267933744</v>
+      </c>
+      <c r="E22" s="118">
+        <v>0.73115211140000003</v>
+      </c>
+      <c r="F22" s="117">
+        <v>665.46228129896804</v>
+      </c>
+      <c r="H22" s="115">
+        <v>125</v>
+      </c>
+      <c r="I22" s="116">
+        <v>0.76891718750000004</v>
+      </c>
+      <c r="J22" s="117">
+        <v>665.46228129896804</v>
+      </c>
+      <c r="K22" s="118">
+        <v>0.77185812499999995</v>
+      </c>
+      <c r="L22" s="117">
+        <v>759.49532332637705</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="112">
+        <v>98</v>
+      </c>
+      <c r="C23" s="119">
+        <v>0.72718792879999905</v>
+      </c>
+      <c r="D23" s="114">
+        <v>668.57862744935505</v>
+      </c>
+      <c r="E23" s="113">
+        <v>0.73327614559999998</v>
+      </c>
+      <c r="F23" s="114">
+        <v>669.09496487444505</v>
+      </c>
+      <c r="H23" s="112">
+        <v>126</v>
+      </c>
+      <c r="I23" s="119">
+        <v>0.76999010639999999</v>
+      </c>
+      <c r="J23" s="114">
+        <v>669.09496487444505</v>
+      </c>
+      <c r="K23" s="113">
+        <v>0.77283707680000002</v>
+      </c>
+      <c r="L23" s="114">
+        <v>762.58984642959194</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="115">
+        <v>99</v>
+      </c>
+      <c r="C24" s="116">
+        <v>0.72948392610000001</v>
+      </c>
+      <c r="D24" s="117">
+        <v>672.18739096161903</v>
+      </c>
+      <c r="E24" s="118">
+        <v>0.73533483820000001</v>
+      </c>
+      <c r="F24" s="117">
+        <v>672.70505600073102</v>
+      </c>
+      <c r="H24" s="115">
+        <v>127</v>
+      </c>
+      <c r="I24" s="116">
+        <v>0.77105501369999996</v>
+      </c>
+      <c r="J24" s="117">
+        <v>672.70505600073102</v>
+      </c>
+      <c r="K24" s="118">
+        <v>0.77380138939999998</v>
+      </c>
+      <c r="L24" s="117">
+        <v>765.668151266015</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="112">
+        <v>100</v>
+      </c>
+      <c r="C25" s="119">
+        <v>0.73170000000000002</v>
+      </c>
+      <c r="D25" s="114">
+        <v>675.77385671651803</v>
+      </c>
+      <c r="E25" s="113">
+        <v>0.73733000000000004</v>
+      </c>
+      <c r="F25" s="114">
+        <v>676.29285284725904</v>
+      </c>
+      <c r="H25" s="112">
+        <v>128</v>
+      </c>
+      <c r="I25" s="119">
+        <v>0.77211457279999995</v>
+      </c>
+      <c r="J25" s="114">
+        <v>676.29285284725904</v>
+      </c>
+      <c r="K25" s="113">
+        <v>0.7747528736</v>
+      </c>
+      <c r="L25" s="114">
+        <v>768.73040765228495</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="115">
+        <v>101</v>
+      </c>
+      <c r="C26" s="116">
+        <v>0.73383881390000005</v>
+      </c>
+      <c r="D26" s="117">
+        <v>679.33831625575704</v>
+      </c>
+      <c r="E26" s="118">
+        <v>0.73926344180000003</v>
+      </c>
+      <c r="F26" s="117">
+        <v>679.85864688085599</v>
+      </c>
+      <c r="H26" s="115">
+        <v>129</v>
+      </c>
+      <c r="I26" s="116">
+        <v>0.77317144709999996</v>
+      </c>
+      <c r="J26" s="117">
+        <v>679.85864688085599</v>
+      </c>
+      <c r="K26" s="118">
+        <v>0.77569334020000003</v>
+      </c>
+      <c r="L26" s="117">
+        <v>771.77678242291404</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="112">
+        <v>102</v>
+      </c>
+      <c r="C27" s="119">
+        <v>0.7359030312</v>
+      </c>
+      <c r="D27" s="114">
+        <v>682.88105463256898</v>
+      </c>
+      <c r="E27" s="113">
+        <v>0.74113697440000004</v>
+      </c>
+      <c r="F27" s="114">
+        <v>683.40272308149304</v>
+      </c>
+      <c r="H27" s="112">
+        <v>130</v>
+      </c>
+      <c r="I27" s="119">
+        <v>0.77422829999999998</v>
+      </c>
+      <c r="J27" s="114">
+        <v>683.40272308149304</v>
+      </c>
+      <c r="K27" s="113">
+        <v>0.7766246</v>
+      </c>
+      <c r="L27" s="114">
+        <v>774.80743950528404</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="115">
+        <v>103</v>
+      </c>
+      <c r="C28" s="116">
+        <v>0.73789531529999997</v>
+      </c>
+      <c r="D28" s="117">
+        <v>686.40235061851195</v>
+      </c>
+      <c r="E28" s="118">
+        <v>0.7429524086</v>
+      </c>
+      <c r="F28" s="117">
+        <v>686.92536014903806</v>
+      </c>
+      <c r="H28" s="115">
+        <v>131</v>
+      </c>
+      <c r="I28" s="116">
+        <v>0.77528779489999999</v>
+      </c>
+      <c r="J28" s="117">
+        <v>686.92536014903806</v>
+      </c>
+      <c r="K28" s="118">
+        <v>0.77754846379999998</v>
+      </c>
+      <c r="L28" s="117">
+        <v>777.82253999219802</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="112">
+        <v>104</v>
+      </c>
+      <c r="C29" s="119">
+        <v>0.73981832960000005</v>
+      </c>
+      <c r="D29" s="114">
+        <v>689.90247690170702</v>
+      </c>
+      <c r="E29" s="113">
+        <v>0.74471155519999999</v>
+      </c>
+      <c r="F29" s="114">
+        <v>690.42683070144597</v>
+      </c>
+      <c r="H29" s="112">
+        <v>132</v>
+      </c>
+      <c r="I29" s="119">
+        <v>0.7763525952</v>
+      </c>
+      <c r="J29" s="114">
+        <v>690.42683070144597</v>
+      </c>
+      <c r="K29" s="113">
+        <v>0.77846674240000002</v>
+      </c>
+      <c r="L29" s="114">
+        <v>780.82224221205797</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="115">
+        <v>105</v>
+      </c>
+      <c r="C30" s="116">
+        <v>0.74167473750000001</v>
+      </c>
+      <c r="D30" s="117">
+        <v>693.38170027696594</v>
+      </c>
+      <c r="E30" s="118">
+        <v>0.74641622500000004</v>
+      </c>
+      <c r="F30" s="117">
+        <v>693.90740146483995</v>
+      </c>
+      <c r="H30" s="115">
+        <v>133</v>
+      </c>
+      <c r="I30" s="116">
+        <v>0.77742536429999998</v>
+      </c>
+      <c r="J30" s="117">
+        <v>693.90740146483995</v>
+      </c>
+      <c r="K30" s="118">
+        <v>0.77938124659999997</v>
+      </c>
+      <c r="L30" s="117">
+        <v>783.80670179680396</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="112">
+        <v>106</v>
+      </c>
+      <c r="C31" s="119">
+        <v>0.74346720239999997</v>
+      </c>
+      <c r="D31" s="114">
+        <v>696.840281828196</v>
+      </c>
+      <c r="E31" s="113">
+        <v>0.74806822880000001</v>
+      </c>
+      <c r="F31" s="114">
+        <v>697.367333455878</v>
+      </c>
+      <c r="H31" s="112">
+        <v>134</v>
+      </c>
+      <c r="I31" s="119">
+        <v>0.77850876560000004</v>
+      </c>
+      <c r="J31" s="114">
+        <v>697.367333455878</v>
+      </c>
+      <c r="K31" s="113">
+        <v>0.78029378719999898</v>
+      </c>
+      <c r="L31" s="114">
+        <v>786.77607174766001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="115">
+        <v>107</v>
+      </c>
+      <c r="C32" s="116">
+        <v>0.74519838770000002</v>
+      </c>
+      <c r="D32" s="117">
+        <v>700.27847710348703</v>
+      </c>
+      <c r="E32" s="118">
+        <v>0.74966937739999995</v>
+      </c>
+      <c r="F32" s="117">
+        <v>700.80688215679197</v>
+      </c>
+      <c r="H32" s="120">
+        <v>135</v>
+      </c>
+      <c r="I32" s="74">
+        <v>0.77960546249999996</v>
+      </c>
+      <c r="J32" s="121">
+        <v>700.80688215679197</v>
+      </c>
+      <c r="K32" s="71">
+        <v>0.781206175</v>
+      </c>
+      <c r="L32" s="121">
+        <v>789.73050249881703</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="112">
+        <v>108</v>
+      </c>
+      <c r="C33" s="119">
+        <v>0.74687095680000004</v>
+      </c>
+      <c r="D33" s="114">
+        <v>703.69653628321998</v>
+      </c>
+      <c r="E33" s="113">
+        <v>0.75122148160000002</v>
+      </c>
+      <c r="F33" s="114">
+        <v>704.22629768347099</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="115">
+        <v>109</v>
+      </c>
+      <c r="C34" s="116">
+        <v>0.74848757310000003</v>
+      </c>
+      <c r="D34" s="117">
+        <v>707.09470434156401</v>
+      </c>
+      <c r="E34" s="118">
+        <v>0.75272635219999995</v>
+      </c>
+      <c r="F34" s="117">
+        <v>707.625824946899</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="112">
+        <v>110</v>
+      </c>
+      <c r="C35" s="119">
+        <v>0.75005089999999996</v>
+      </c>
+      <c r="D35" s="114">
+        <v>710.47322120164199</v>
+      </c>
+      <c r="E35" s="113">
+        <v>0.75418580000000002</v>
+      </c>
+      <c r="F35" s="114">
+        <v>711.00570380830504</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="115">
+        <v>111</v>
+      </c>
+      <c r="C36" s="116">
+        <v>0.75156360089999996</v>
+      </c>
+      <c r="D36" s="117">
+        <v>713.83232188471095</v>
+      </c>
+      <c r="E36" s="118">
+        <v>0.75560163579999995</v>
+      </c>
+      <c r="F36" s="117">
+        <v>714.36616922829205</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="112">
+        <v>112</v>
+      </c>
+      <c r="C37" s="119">
+        <v>0.75302833920000001</v>
+      </c>
+      <c r="D37" s="114">
+        <v>717.17223665360802</v>
+      </c>
+      <c r="E37" s="113">
+        <v>0.75697567040000002</v>
+      </c>
+      <c r="F37" s="114">
+        <v>717.70745141025998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="115">
+        <v>113</v>
+      </c>
+      <c r="C38" s="116">
+        <v>0.75444777829999998</v>
+      </c>
+      <c r="D38" s="117">
+        <v>720.49319115075298</v>
+      </c>
+      <c r="E38" s="118">
+        <v>0.75830971459999996</v>
+      </c>
+      <c r="F38" s="117">
+        <v>721.02977593836795</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="112">
+        <v>114</v>
+      </c>
+      <c r="C39" s="119">
+        <v>0.75582458159999999</v>
+      </c>
+      <c r="D39" s="114">
+        <v>723.79540653094296</v>
+      </c>
+      <c r="E39" s="113">
+        <v>0.75960557920000005</v>
+      </c>
+      <c r="F39" s="114">
+        <v>724.333363910304</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="115">
+        <v>115</v>
+      </c>
+      <c r="C40" s="116">
+        <v>0.75716141250000002</v>
+      </c>
+      <c r="D40" s="117">
+        <v>727.07909958920095</v>
+      </c>
+      <c r="E40" s="118">
+        <v>0.760865075</v>
+      </c>
+      <c r="F40" s="117">
+        <v>727.618432065094</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="112">
+        <v>116</v>
+      </c>
+      <c r="C41" s="119">
+        <v>0.75846093439999995</v>
+      </c>
+      <c r="D41" s="114">
+        <v>730.34448288387898</v>
+      </c>
+      <c r="E41" s="113">
+        <v>0.76209001279999999</v>
+      </c>
+      <c r="F41" s="114">
+        <v>730.88519290618603</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="115">
+        <v>117</v>
+      </c>
+      <c r="C42" s="116">
+        <v>0.7597258107</v>
+      </c>
+      <c r="D42" s="117">
+        <v>733.59176485525597</v>
+      </c>
+      <c r="E42" s="118">
+        <v>0.76328220339999997</v>
+      </c>
+      <c r="F42" s="117">
+        <v>734.13385482000797</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="112">
+        <v>118</v>
+      </c>
+      <c r="C43" s="119">
+        <v>0.76095870480000005</v>
+      </c>
+      <c r="D43" s="114">
+        <v>736.821149939816</v>
+      </c>
+      <c r="E43" s="113">
+        <v>0.76444345759999999</v>
+      </c>
+      <c r="F43" s="114">
+        <v>737.36462219023304</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="115">
+        <v>119</v>
+      </c>
+      <c r="C44" s="116">
+        <v>0.76216228009999998</v>
+      </c>
+      <c r="D44" s="117">
+        <v>740.03283868040603</v>
+      </c>
+      <c r="E44" s="118">
+        <v>0.76557558619999999</v>
+      </c>
+      <c r="F44" s="117">
+        <v>740.57769550789601</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="112">
+        <v>120</v>
+      </c>
+      <c r="C45" s="119">
+        <v>0.7633392</v>
+      </c>
+      <c r="D45" s="114">
+        <v>743.22702783246098</v>
+      </c>
+      <c r="E45" s="113">
+        <v>0.76668040000000004</v>
+      </c>
+      <c r="F45" s="114">
+        <v>743.77327147760195</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="115">
+        <v>121</v>
+      </c>
+      <c r="C46" s="116">
+        <v>0.76449212789999998</v>
+      </c>
+      <c r="D46" s="117">
+        <v>746.40391046645198</v>
+      </c>
+      <c r="E46" s="118">
+        <v>0.76775970979999997</v>
+      </c>
+      <c r="F46" s="117">
+        <v>746.95154311994702</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="112">
+        <v>122</v>
+      </c>
+      <c r="C47" s="119">
+        <v>0.76562372720000005</v>
+      </c>
+      <c r="D47" s="114">
+        <v>749.56367606673803</v>
+      </c>
+      <c r="E47" s="113">
+        <v>0.76881532640000005</v>
+      </c>
+      <c r="F47" s="114">
+        <v>750.11269987034495</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="115">
+        <v>123</v>
+      </c>
+      <c r="C48" s="116">
+        <v>0.76673666129999996</v>
+      </c>
+      <c r="D48" s="117">
+        <v>752.70651062697505</v>
+      </c>
+      <c r="E48" s="118">
+        <v>0.76984906060000002</v>
+      </c>
+      <c r="F48" s="117">
+        <v>753.25692767441399</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="112">
+        <v>124</v>
+      </c>
+      <c r="C49" s="119">
+        <v>0.76783359360000003</v>
+      </c>
+      <c r="D49" s="114">
+        <v>755.83259674221597</v>
+      </c>
+      <c r="E49" s="113">
+        <v>0.77086272319999904</v>
+      </c>
+      <c r="F49" s="114">
+        <v>756.384409080056</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="115">
+        <v>125</v>
+      </c>
+      <c r="C50" s="116">
+        <v>0.76891718750000004</v>
+      </c>
+      <c r="D50" s="117">
+        <v>758.94211369785705</v>
+      </c>
+      <c r="E50" s="118">
+        <v>0.77185812499999995</v>
+      </c>
+      <c r="F50" s="117">
+        <v>759.49532332637705</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="112">
+        <v>126</v>
+      </c>
+      <c r="C51" s="119">
+        <v>0.76999010639999999</v>
+      </c>
+      <c r="D51" s="114">
+        <v>762.03523755555898</v>
+      </c>
+      <c r="E51" s="113">
+        <v>0.77283707680000002</v>
+      </c>
+      <c r="F51" s="114">
+        <v>762.58984642959194</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="115">
+        <v>127</v>
+      </c>
+      <c r="C52" s="116">
+        <v>0.77105501369999996</v>
+      </c>
+      <c r="D52" s="117">
+        <v>765.11214123626098</v>
+      </c>
+      <c r="E52" s="118">
+        <v>0.77380138939999998</v>
+      </c>
+      <c r="F52" s="117">
+        <v>765.668151266015</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="112">
+        <v>128</v>
+      </c>
+      <c r="C53" s="119">
+        <v>0.77211457279999995</v>
+      </c>
+      <c r="D53" s="114">
+        <v>768.17299460042295</v>
+      </c>
+      <c r="E53" s="113">
+        <v>0.7747528736</v>
+      </c>
+      <c r="F53" s="114">
+        <v>768.73040765228495</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="115">
+        <v>129</v>
+      </c>
+      <c r="C54" s="116">
+        <v>0.77317144709999996</v>
+      </c>
+      <c r="D54" s="117">
+        <v>771.21796452559602</v>
+      </c>
+      <c r="E54" s="118">
+        <v>0.77569334020000003</v>
+      </c>
+      <c r="F54" s="117">
+        <v>771.77678242291404</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="112">
+        <v>130</v>
+      </c>
+      <c r="C55" s="119">
+        <v>0.77422829999999998</v>
+      </c>
+      <c r="D55" s="114">
+        <v>774.24721498144095</v>
+      </c>
+      <c r="E55" s="113">
+        <v>0.7766246</v>
+      </c>
+      <c r="F55" s="114">
+        <v>774.80743950528404</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="115">
+        <v>131</v>
+      </c>
+      <c r="C56" s="116">
+        <v>0.77528779489999999</v>
+      </c>
+      <c r="D56" s="117">
+        <v>777.26090710228402</v>
+      </c>
+      <c r="E56" s="118">
+        <v>0.77754846379999998</v>
+      </c>
+      <c r="F56" s="117">
+        <v>777.82253999219802</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="112">
+        <v>132</v>
+      </c>
+      <c r="C57" s="119">
+        <v>0.7763525952</v>
+      </c>
+      <c r="D57" s="114">
+        <v>780.25919925732796</v>
+      </c>
+      <c r="E57" s="113">
+        <v>0.77846674240000002</v>
+      </c>
+      <c r="F57" s="114">
+        <v>780.82224221205797</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="115">
+        <v>133</v>
+      </c>
+      <c r="C58" s="116">
+        <v>0.77742536429999998</v>
+      </c>
+      <c r="D58" s="117">
+        <v>783.24224711859904</v>
+      </c>
+      <c r="E58" s="118">
+        <v>0.77938124659999997</v>
+      </c>
+      <c r="F58" s="117">
+        <v>783.80670179680396</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="112">
+        <v>134</v>
+      </c>
+      <c r="C59" s="119">
+        <v>0.77850876560000004</v>
+      </c>
+      <c r="D59" s="114">
+        <v>786.21020372671296</v>
+      </c>
+      <c r="E59" s="113">
+        <v>0.78029378719999898</v>
+      </c>
+      <c r="F59" s="114">
+        <v>786.77607174766001</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="120">
+        <v>135</v>
+      </c>
+      <c r="C60" s="74">
+        <v>0.77960546249999996</v>
+      </c>
+      <c r="D60" s="121">
+        <v>789.16321955456897</v>
+      </c>
+      <c r="E60" s="71">
+        <v>0.781206175</v>
+      </c>
+      <c r="F60" s="121">
+        <v>789.73050249881703</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="I2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E624D2-11D3-404C-928A-497DC4841E45}">
+  <dimension ref="B1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5940,46 +7724,64 @@
     <col min="2" max="2" width="7.140625" style="23" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="25" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="28" customWidth="1"/>
-    <col min="7" max="7" width="1.42578125" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="77" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="10" style="28" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="68" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="72"/>
-      <c r="C3" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="61" t="s">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="95"/>
+      <c r="C2" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="63"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="63"/>
-      <c r="K3" s="61" t="s">
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+      <c r="L2" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="63"/>
-    </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="99"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="96"/>
+      <c r="C3" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="92"/>
+      <c r="G3" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="92"/>
+      <c r="I3" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="92"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="54" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E4" s="56" t="s">
         <v>14</v>
@@ -5987,765 +7789,1372 @@
       <c r="F4" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="54" t="s">
-        <v>13</v>
+      <c r="G4" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>46</v>
       </c>
       <c r="I4" s="56" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J4" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="59" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="73">
-        <v>80</v>
-      </c>
-      <c r="C5" s="74">
-        <v>0.68313307999999995</v>
-      </c>
-      <c r="D5" s="75">
-        <v>600.40592741891703</v>
-      </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="30">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="64">
+        <v>82</v>
+      </c>
+      <c r="C5" s="65">
+        <v>0.69005955712</v>
+      </c>
+      <c r="D5" s="66">
+        <v>608.51325914511403</v>
+      </c>
+      <c r="E5" s="65"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
+        <v>0.69005955712</v>
+      </c>
+      <c r="H5" s="66">
+        <v>608.51325914511403</v>
+      </c>
+      <c r="I5" s="65">
+        <v>0.69</v>
+      </c>
+      <c r="J5" s="67">
+        <v>606.6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="30">
+        <v>83</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0.69338047808000003</v>
+      </c>
+      <c r="D6" s="28">
+        <v>612.52395801226805</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="25">
+        <v>0.69338047808000003</v>
+      </c>
+      <c r="H6" s="28">
+        <v>612.52395801226805</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="35">
+        <v>84</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0.69660893535999902</v>
+      </c>
+      <c r="D7" s="61">
+        <v>616.50660894770101</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="37">
+        <v>0.69660893535999902</v>
+      </c>
+      <c r="H7" s="61">
+        <v>616.50660894770101</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="30">
+        <v>85</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0.69974674000000003</v>
+      </c>
+      <c r="D8" s="28">
+        <v>620.46164449986202</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="25">
+        <v>0.69974674000000003</v>
+      </c>
+      <c r="H8" s="28">
+        <v>620.46164449986202</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="35">
+        <v>86</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0.70279570304000005</v>
+      </c>
+      <c r="D9" s="61">
+        <v>624.389485768697</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="37">
+        <v>0.70279570304000005</v>
+      </c>
+      <c r="H9" s="61">
+        <v>624.389485768697</v>
+      </c>
+      <c r="I9" s="37"/>
+      <c r="J9" s="38"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="30">
+        <v>87</v>
+      </c>
+      <c r="C10" s="25">
+        <v>0.70575763552000004</v>
+      </c>
+      <c r="D10" s="28">
+        <v>628.29054283907601</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="25">
+        <v>0.70575763552000004</v>
+      </c>
+      <c r="H10" s="28">
+        <v>628.29054283907601</v>
+      </c>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="35">
+        <v>88</v>
+      </c>
+      <c r="C11" s="37">
+        <v>0.70863434847999995</v>
+      </c>
+      <c r="D11" s="61">
+        <v>632.16521519297896</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="37">
+        <v>0.70863434847999995</v>
+      </c>
+      <c r="H11" s="61">
+        <v>632.16521519297896</v>
+      </c>
+      <c r="I11" s="37"/>
+      <c r="J11" s="38"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="30">
+        <v>89</v>
+      </c>
+      <c r="C12" s="25">
+        <v>0.71142765295999999</v>
+      </c>
+      <c r="D12" s="28">
+        <v>636.01389210171305</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="25">
+        <v>0.71142765295999999</v>
+      </c>
+      <c r="H12" s="28">
+        <v>636.01389210171305</v>
+      </c>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="35">
+        <v>90</v>
+      </c>
+      <c r="C13" s="37">
+        <v>0.71413936</v>
+      </c>
+      <c r="D13" s="61">
+        <v>639.83695299932697</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="37">
+        <v>0.71413936</v>
+      </c>
+      <c r="H13" s="61">
+        <v>639.83695299932697</v>
+      </c>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="30">
+        <v>91</v>
+      </c>
+      <c r="C14" s="25">
+        <v>0.71677128063999995</v>
+      </c>
+      <c r="D14" s="28">
+        <v>643.63476783834403</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="25">
+        <v>0.71677128063999995</v>
+      </c>
+      <c r="H14" s="28">
+        <v>643.63476783834403</v>
+      </c>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="35">
+        <v>92</v>
+      </c>
+      <c r="C15" s="37">
+        <v>0.71932522592000003</v>
+      </c>
+      <c r="D15" s="61">
+        <v>647.40769742883504</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="37">
+        <v>0.71932522592000003</v>
+      </c>
+      <c r="H15" s="61">
+        <v>647.40769742883504</v>
+      </c>
+      <c r="I15" s="37"/>
+      <c r="J15" s="38"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="30">
+        <v>93</v>
+      </c>
+      <c r="C16" s="25">
+        <v>0.72180300687999999</v>
+      </c>
+      <c r="D16" s="28">
+        <v>651.15609376176496</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="25">
+        <v>0.72180300687999999</v>
+      </c>
+      <c r="H16" s="28">
+        <v>651.15609376176496</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="35">
+        <v>94</v>
+      </c>
+      <c r="C17" s="37">
+        <v>0.72420643456</v>
+      </c>
+      <c r="D17" s="61">
+        <v>654.88030031752999</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="37">
+        <v>0.72420643456</v>
+      </c>
+      <c r="H17" s="61">
+        <v>654.88030031752999</v>
+      </c>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="30">
+        <v>95</v>
+      </c>
+      <c r="C18" s="25">
+        <v>0.72653732000000004</v>
+      </c>
+      <c r="D18" s="28">
+        <v>658.580652360503</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="25">
+        <v>0.72653732000000004</v>
+      </c>
+      <c r="H18" s="28">
+        <v>658.580652360503</v>
+      </c>
+      <c r="I18" s="25">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="J18" s="26">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="35">
+        <v>96</v>
+      </c>
+      <c r="C19" s="37">
+        <v>0.72879747423999997</v>
+      </c>
+      <c r="D19" s="61">
+        <v>662.25747722035896</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="37">
+        <v>0.72879747423999997</v>
+      </c>
+      <c r="H19" s="61">
+        <v>662.25747722035896</v>
+      </c>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="30">
+        <v>97</v>
+      </c>
+      <c r="C20" s="25">
+        <v>0.73098870831999996</v>
+      </c>
+      <c r="D20" s="28">
+        <v>665.91109456091897</v>
+      </c>
+      <c r="F20" s="26"/>
+      <c r="G20" s="25">
+        <v>0.73098870831999996</v>
+      </c>
+      <c r="H20" s="28">
+        <v>665.91109456091897</v>
+      </c>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="35">
+        <v>98</v>
+      </c>
+      <c r="C21" s="37">
+        <v>0.73311283327999999</v>
+      </c>
+      <c r="D21" s="61">
+        <v>669.54181663717804</v>
+      </c>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="37">
+        <v>0.73311283327999999</v>
+      </c>
+      <c r="H21" s="61">
+        <v>669.54181663717804</v>
+      </c>
+      <c r="I21" s="37"/>
+      <c r="J21" s="38"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="30">
+        <v>99</v>
+      </c>
+      <c r="C22" s="25">
+        <v>0.73517166015999902</v>
+      </c>
+      <c r="D22" s="28">
+        <v>673.14994854116003</v>
+      </c>
+      <c r="F22" s="26"/>
+      <c r="G22" s="25">
+        <v>0.73517166015999902</v>
+      </c>
+      <c r="H22" s="28">
+        <v>673.14994854116003</v>
+      </c>
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="35">
+        <v>100</v>
+      </c>
+      <c r="C23" s="37">
+        <v>0.73716700000000002</v>
+      </c>
+      <c r="D23" s="61">
+        <v>676.73578843719201</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="37">
+        <v>0.73716700000000002</v>
+      </c>
+      <c r="H23" s="61">
+        <v>676.73578843719201</v>
+      </c>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="30">
+        <v>101</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0.73910066383999995</v>
+      </c>
+      <c r="D24" s="28">
+        <v>680.29962778714696</v>
+      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="25">
+        <v>0.73910066383999995</v>
+      </c>
+      <c r="H24" s="28">
+        <v>680.29962778714696</v>
+      </c>
+      <c r="I24" s="25"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="35">
+        <v>102</v>
+      </c>
+      <c r="C25" s="37">
+        <v>0.74097446272</v>
+      </c>
+      <c r="D25" s="61">
+        <v>683.84175156620404</v>
+      </c>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="37">
+        <v>0.74097446272</v>
+      </c>
+      <c r="H25" s="61">
+        <v>683.84175156620404</v>
+      </c>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="30">
+        <v>103</v>
+      </c>
+      <c r="C26" s="25">
+        <v>0.74279020768000004</v>
+      </c>
+      <c r="D26" s="28">
+        <v>687.36243846957098</v>
+      </c>
+      <c r="F26" s="26"/>
+      <c r="G26" s="25">
+        <v>0.74279020768000004</v>
+      </c>
+      <c r="H26" s="28">
+        <v>687.36243846957098</v>
+      </c>
+      <c r="I26" s="25"/>
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="35">
+        <v>104</v>
+      </c>
+      <c r="C27" s="37">
+        <v>0.74454970976000001</v>
+      </c>
+      <c r="D27" s="61">
+        <v>690.86196111068398</v>
+      </c>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="37">
+        <v>0.74454970976000001</v>
+      </c>
+      <c r="H27" s="61">
+        <v>690.86196111068398</v>
+      </c>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="30">
+        <v>105</v>
+      </c>
+      <c r="C28" s="25">
+        <v>0.74625478000000001</v>
+      </c>
+      <c r="D28" s="28">
+        <v>694.34058621127701</v>
+      </c>
+      <c r="F28" s="26"/>
+      <c r="G28" s="25">
+        <v>0.74625478000000001</v>
+      </c>
+      <c r="H28" s="28">
+        <v>694.34058621127701</v>
+      </c>
+      <c r="I28" s="25"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="35">
+        <v>106</v>
+      </c>
+      <c r="C29" s="37">
+        <v>0.74790722943999899</v>
+      </c>
+      <c r="D29" s="61">
+        <v>697.79857478373799</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="37">
+        <v>0.74790722943999899</v>
+      </c>
+      <c r="H29" s="61">
+        <v>697.79857478373799</v>
+      </c>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="30">
+        <v>107</v>
+      </c>
+      <c r="C30" s="25">
+        <v>0.74950886912000003</v>
+      </c>
+      <c r="D30" s="28">
+        <v>701.23618230614795</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="25">
+        <v>0.74950886912000003</v>
+      </c>
+      <c r="H30" s="28">
+        <v>701.23618230614795</v>
+      </c>
+      <c r="I30" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J30" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="35">
+        <v>108</v>
+      </c>
+      <c r="C31" s="37">
+        <v>0.75106151007999999</v>
+      </c>
+      <c r="D31" s="61">
+        <v>704.65365889035195</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="37">
+        <v>0.75106151007999999</v>
+      </c>
+      <c r="H31" s="61">
+        <v>704.65365889035195</v>
+      </c>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="30">
         <v>109</v>
       </c>
-      <c r="I5" s="69">
-        <v>0.75256696335999995</v>
-      </c>
-      <c r="J5" s="70">
-        <v>708.05124944339502</v>
-      </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="26"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="30">
-        <v>81</v>
-      </c>
-      <c r="C6" s="69">
-        <v>0.68664436143999996</v>
-      </c>
-      <c r="D6" s="70">
-        <v>604.47406789322997</v>
-      </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="35">
+      <c r="C32" s="25">
+        <v>0.75261415103999996</v>
+      </c>
+      <c r="D32" s="28">
+        <v>708.07113547455594</v>
+      </c>
+      <c r="F32" s="26"/>
+      <c r="G32" s="25">
+        <v>0.75261415103999996</v>
+      </c>
+      <c r="H32" s="28">
+        <v>708.07113547455594</v>
+      </c>
+      <c r="I32" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J32" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="35">
         <v>110</v>
       </c>
-      <c r="I6" s="66">
-        <v>0.75402703999999998</v>
-      </c>
-      <c r="J6" s="67">
-        <v>711.42919382266496</v>
-      </c>
-      <c r="K6" s="66"/>
-      <c r="L6" s="38"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="35">
-        <v>82</v>
-      </c>
-      <c r="C7" s="66">
-        <v>0.69005955712</v>
-      </c>
-      <c r="D7" s="67">
-        <v>608.51325914511403</v>
-      </c>
-      <c r="E7" s="66">
-        <v>0.69</v>
-      </c>
-      <c r="F7" s="38">
-        <v>606.6</v>
-      </c>
-      <c r="G7" s="68"/>
-      <c r="H7" s="30">
+      <c r="C33" s="37">
+        <v>0.75416679200000003</v>
+      </c>
+      <c r="D33" s="61">
+        <v>711.48861205876005</v>
+      </c>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="37">
+        <v>0.75416679200000003</v>
+      </c>
+      <c r="H33" s="61">
+        <v>711.48861205876005</v>
+      </c>
+      <c r="I33" s="37"/>
+      <c r="J33" s="38"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="30">
         <v>111</v>
       </c>
-      <c r="I7" s="69">
-        <v>0.75544355104000005</v>
-      </c>
-      <c r="J7" s="70">
-        <v>714.78772698502098</v>
-      </c>
-      <c r="K7" s="69"/>
-      <c r="L7" s="26"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="30">
-        <v>83</v>
-      </c>
-      <c r="C8" s="69">
-        <v>0.69338047808000003</v>
-      </c>
-      <c r="D8" s="70">
-        <v>612.52395801226805</v>
-      </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="35">
+      <c r="C34" s="25">
+        <v>0.75571943295999999</v>
+      </c>
+      <c r="D34" s="28">
+        <v>714.90608864296405</v>
+      </c>
+      <c r="F34" s="26"/>
+      <c r="G34" s="25">
+        <v>0.75571943295999999</v>
+      </c>
+      <c r="H34" s="28">
+        <v>714.90608864296405</v>
+      </c>
+      <c r="I34" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J34" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="35">
         <v>112</v>
       </c>
-      <c r="I8" s="66">
-        <v>0.75681830752000001</v>
-      </c>
-      <c r="J8" s="67">
-        <v>718.12707913020404</v>
-      </c>
-      <c r="K8" s="66"/>
-      <c r="L8" s="38"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="35">
-        <v>84</v>
-      </c>
-      <c r="C9" s="66">
-        <v>0.69660893535999902</v>
-      </c>
-      <c r="D9" s="67">
-        <v>616.50660894770101</v>
-      </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="30">
+      <c r="C35" s="37">
+        <v>0.75727207391999996</v>
+      </c>
+      <c r="D35" s="61">
+        <v>718.32356522716805</v>
+      </c>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="37">
+        <v>0.75727207391999996</v>
+      </c>
+      <c r="H35" s="61">
+        <v>718.32356522716805</v>
+      </c>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="30">
         <v>113</v>
       </c>
-      <c r="I9" s="69">
-        <v>0.75815312047999905</v>
-      </c>
-      <c r="J9" s="70">
-        <v>721.44747583880201</v>
-      </c>
-      <c r="K9" s="69"/>
-      <c r="L9" s="26"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="30">
-        <v>85</v>
-      </c>
-      <c r="C10" s="69">
-        <v>0.69974674000000003</v>
-      </c>
-      <c r="D10" s="70">
-        <v>620.46164449986202</v>
-      </c>
-      <c r="E10" s="69"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="35">
+      <c r="C36" s="25">
+        <v>0.75882471488000003</v>
+      </c>
+      <c r="D36" s="28">
+        <v>721.74104181137204</v>
+      </c>
+      <c r="F36" s="26"/>
+      <c r="G36" s="25">
+        <v>0.75882471488000003</v>
+      </c>
+      <c r="H36" s="28">
+        <v>721.74104181137204</v>
+      </c>
+      <c r="I36" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J36" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="35">
         <v>114</v>
       </c>
-      <c r="I10" s="66">
-        <v>0.75944980096000003</v>
-      </c>
-      <c r="J10" s="67">
-        <v>724.74913820500899</v>
-      </c>
-      <c r="K10" s="66"/>
-      <c r="L10" s="38"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="35">
-        <v>86</v>
-      </c>
-      <c r="C11" s="66">
-        <v>0.70279570304000005</v>
-      </c>
-      <c r="D11" s="67">
-        <v>624.389485768697</v>
-      </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="30">
+      <c r="C37" s="37">
+        <v>0.76037735583999999</v>
+      </c>
+      <c r="D37" s="61">
+        <v>725.15851839557604</v>
+      </c>
+      <c r="E37" s="37"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="37">
+        <v>0.76037735583999999</v>
+      </c>
+      <c r="H37" s="61">
+        <v>725.15851839557604</v>
+      </c>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="30">
         <v>115</v>
       </c>
-      <c r="I11" s="69">
-        <v>0.76071016000000002</v>
-      </c>
-      <c r="J11" s="70">
-        <v>728.03228296443501</v>
-      </c>
-      <c r="K11" s="69"/>
-      <c r="L11" s="26"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="30">
-        <v>87</v>
-      </c>
-      <c r="C12" s="69">
-        <v>0.70575763552000004</v>
-      </c>
-      <c r="D12" s="70">
-        <v>628.29054283907601</v>
-      </c>
-      <c r="E12" s="69"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="35">
+      <c r="C38" s="25">
+        <v>0.76192999679999995</v>
+      </c>
+      <c r="D38" s="28">
+        <v>728.57599497978003</v>
+      </c>
+      <c r="F38" s="26"/>
+      <c r="G38" s="25">
+        <v>0.76192999679999995</v>
+      </c>
+      <c r="H38" s="28">
+        <v>728.57599497978003</v>
+      </c>
+      <c r="I38" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J38" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="35">
         <v>116</v>
       </c>
-      <c r="I12" s="66">
-        <v>0.761936008639999</v>
-      </c>
-      <c r="J12" s="67">
-        <v>731.29712261718203</v>
-      </c>
-      <c r="K12" s="66"/>
-      <c r="L12" s="38"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="35">
-        <v>88</v>
-      </c>
-      <c r="C13" s="66">
-        <v>0.70863434847999995</v>
-      </c>
-      <c r="D13" s="67">
-        <v>632.16521519297896</v>
-      </c>
-      <c r="E13" s="66"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="30">
+      <c r="C39" s="37">
+        <v>0.76348263776000003</v>
+      </c>
+      <c r="D39" s="61">
+        <v>731.99347156398403</v>
+      </c>
+      <c r="E39" s="37"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="37">
+        <v>0.76348263776000003</v>
+      </c>
+      <c r="H39" s="61">
+        <v>731.99347156398403</v>
+      </c>
+      <c r="I39" s="37"/>
+      <c r="J39" s="38"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="30">
         <v>117</v>
       </c>
-      <c r="I13" s="69">
-        <v>0.76312915792000002</v>
-      </c>
-      <c r="J13" s="70">
-        <v>734.54386554640701</v>
-      </c>
-      <c r="K13" s="69"/>
-      <c r="L13" s="26"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="30">
-        <v>89</v>
-      </c>
-      <c r="C14" s="69">
-        <v>0.71142765295999999</v>
-      </c>
-      <c r="D14" s="70">
-        <v>636.01389210171305</v>
-      </c>
-      <c r="E14" s="69"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="35">
+      <c r="C40" s="25">
+        <v>0.76503527871999999</v>
+      </c>
+      <c r="D40" s="28">
+        <v>735.41094814818803</v>
+      </c>
+      <c r="F40" s="26"/>
+      <c r="G40" s="25">
+        <v>0.76503527871999999</v>
+      </c>
+      <c r="H40" s="28">
+        <v>735.41094814818803</v>
+      </c>
+      <c r="I40" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J40" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="35">
         <v>118</v>
       </c>
-      <c r="I14" s="66">
-        <v>0.76429141887999996</v>
-      </c>
-      <c r="J14" s="67">
-        <v>737.77271613256801</v>
-      </c>
-      <c r="K14" s="66"/>
-      <c r="L14" s="38"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="35">
-        <v>90</v>
-      </c>
-      <c r="C15" s="66">
-        <v>0.71413936</v>
-      </c>
-      <c r="D15" s="67">
-        <v>639.83695299932697</v>
-      </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="30">
+      <c r="C41" s="37">
+        <v>0.76658791967999995</v>
+      </c>
+      <c r="D41" s="61">
+        <v>738.82842473239202</v>
+      </c>
+      <c r="E41" s="37"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="37">
+        <v>0.76658791967999995</v>
+      </c>
+      <c r="H41" s="61">
+        <v>738.82842473239202</v>
+      </c>
+      <c r="I41" s="37"/>
+      <c r="J41" s="38"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="30">
         <v>119</v>
       </c>
-      <c r="I15" s="69">
-        <v>0.76542460256</v>
-      </c>
-      <c r="J15" s="70">
-        <v>740.98387486355296</v>
-      </c>
-      <c r="K15" s="69"/>
-      <c r="L15" s="26"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="30">
-        <v>91</v>
-      </c>
-      <c r="C16" s="69">
-        <v>0.71677128063999995</v>
-      </c>
-      <c r="D16" s="70">
-        <v>643.63476783834403</v>
-      </c>
-      <c r="E16" s="69"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="35">
+      <c r="C42" s="25">
+        <v>0.76814056064000003</v>
+      </c>
+      <c r="D42" s="28">
+        <v>742.24590131659602</v>
+      </c>
+      <c r="F42" s="26"/>
+      <c r="G42" s="25">
+        <v>0.76814056064000003</v>
+      </c>
+      <c r="H42" s="28">
+        <v>742.24590131659602</v>
+      </c>
+      <c r="I42" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J42" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="35">
         <v>120</v>
       </c>
-      <c r="I16" s="66">
-        <v>0.76653051999999999</v>
-      </c>
-      <c r="J16" s="67">
-        <v>744.17753844087599</v>
-      </c>
-      <c r="K16" s="66"/>
-      <c r="L16" s="38"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
-        <v>92</v>
-      </c>
-      <c r="C17" s="66">
-        <v>0.71932522592000003</v>
-      </c>
-      <c r="D17" s="67">
-        <v>647.40769742883504</v>
-      </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="30">
+      <c r="C43" s="37">
+        <v>0.76969320159999999</v>
+      </c>
+      <c r="D43" s="61">
+        <v>745.66337790080001</v>
+      </c>
+      <c r="E43" s="37"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="37">
+        <v>0.76969320159999999</v>
+      </c>
+      <c r="H43" s="61">
+        <v>745.66337790080001</v>
+      </c>
+      <c r="I43" s="37"/>
+      <c r="J43" s="38"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="30">
         <v>121</v>
       </c>
-      <c r="I17" s="69">
-        <v>0.76761098223999902</v>
-      </c>
-      <c r="J17" s="70">
-        <v>747.35389988209704</v>
-      </c>
-      <c r="K17" s="69">
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="L17" s="26">
-        <v>748.8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="30">
-        <v>93</v>
-      </c>
-      <c r="C18" s="69">
-        <v>0.72180300687999999</v>
-      </c>
-      <c r="D18" s="70">
-        <v>651.15609376176496</v>
-      </c>
-      <c r="E18" s="69"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="35">
+      <c r="C44" s="25">
+        <v>0.77124584255999995</v>
+      </c>
+      <c r="D44" s="28">
+        <v>749.08085448500401</v>
+      </c>
+      <c r="F44" s="26"/>
+      <c r="G44" s="25">
+        <v>0.77124584255999995</v>
+      </c>
+      <c r="H44" s="28">
+        <v>749.08085448500401</v>
+      </c>
+      <c r="I44" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J44" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="35">
         <v>122</v>
       </c>
-      <c r="I18" s="66">
-        <v>0.76866780032000004</v>
-      </c>
-      <c r="J18" s="67">
-        <v>750.51314861964897</v>
-      </c>
-      <c r="K18" s="66"/>
-      <c r="L18" s="38"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="35">
-        <v>94</v>
-      </c>
-      <c r="C19" s="66">
-        <v>0.72420643456</v>
-      </c>
-      <c r="D19" s="67">
-        <v>654.88030031752999</v>
-      </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="30">
+      <c r="C45" s="37">
+        <v>0.77279848351999902</v>
+      </c>
+      <c r="D45" s="61">
+        <v>752.49833106920801</v>
+      </c>
+      <c r="E45" s="37"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="37">
+        <v>0.77279848351999902</v>
+      </c>
+      <c r="H45" s="61">
+        <v>752.49833106920801</v>
+      </c>
+      <c r="I45" s="37"/>
+      <c r="J45" s="38"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="30">
         <v>123</v>
       </c>
-      <c r="I19" s="69">
-        <v>0.76970278527999902</v>
-      </c>
-      <c r="J19" s="70">
-        <v>753.65547059621895</v>
-      </c>
-      <c r="K19" s="69"/>
-      <c r="L19" s="26"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="30">
-        <v>95</v>
-      </c>
-      <c r="C20" s="69">
-        <v>0.72653732000000004</v>
-      </c>
-      <c r="D20" s="70">
-        <v>658.580652360503</v>
-      </c>
-      <c r="E20" s="69">
-        <v>0.72699999999999998</v>
-      </c>
-      <c r="F20" s="26">
-        <v>657</v>
-      </c>
-      <c r="G20" s="68"/>
-      <c r="H20" s="35">
+      <c r="C46" s="25">
+        <v>0.77435112447999899</v>
+      </c>
+      <c r="D46" s="28">
+        <v>755.915807653412</v>
+      </c>
+      <c r="F46" s="26"/>
+      <c r="G46" s="25">
+        <v>0.77435112447999899</v>
+      </c>
+      <c r="H46" s="28">
+        <v>755.915807653412</v>
+      </c>
+      <c r="I46" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J46" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="35">
         <v>124</v>
       </c>
-      <c r="I20" s="66">
-        <v>0.77071774816000005</v>
-      </c>
-      <c r="J20" s="67">
-        <v>756.781048356822</v>
-      </c>
-      <c r="K20" s="66"/>
-      <c r="L20" s="38"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="35">
-        <v>96</v>
-      </c>
-      <c r="C21" s="66">
-        <v>0.72879747423999997</v>
-      </c>
-      <c r="D21" s="67">
-        <v>662.25747722035896</v>
-      </c>
-      <c r="E21" s="66"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="30">
+      <c r="C47" s="37">
+        <v>0.77590376543999895</v>
+      </c>
+      <c r="D47" s="61">
+        <v>759.333284237616</v>
+      </c>
+      <c r="E47" s="37"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="37">
+        <v>0.77590376543999895</v>
+      </c>
+      <c r="H47" s="61">
+        <v>759.333284237616</v>
+      </c>
+      <c r="I47" s="37"/>
+      <c r="J47" s="38"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="30">
         <v>125</v>
       </c>
-      <c r="I21" s="69">
-        <v>0.77171449999999997</v>
-      </c>
-      <c r="J21" s="70">
-        <v>759.89006113772496</v>
-      </c>
-      <c r="K21" s="69"/>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="30">
-        <v>97</v>
-      </c>
-      <c r="C22" s="69">
-        <v>0.73098870831999996</v>
-      </c>
-      <c r="D22" s="70">
-        <v>665.91109456091897</v>
-      </c>
-      <c r="E22" s="69"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="35">
+      <c r="C48" s="25">
+        <v>0.77745640639999902</v>
+      </c>
+      <c r="D48" s="28">
+        <v>762.75076082181999</v>
+      </c>
+      <c r="F48" s="26"/>
+      <c r="G48" s="25">
+        <v>0.77745640639999902</v>
+      </c>
+      <c r="H48" s="28">
+        <v>762.75076082181999</v>
+      </c>
+      <c r="I48" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J48" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="35">
         <v>126</v>
       </c>
-      <c r="I22" s="66">
-        <v>0.77269485183999898</v>
-      </c>
-      <c r="J22" s="67">
-        <v>762.98268495234697</v>
-      </c>
-      <c r="K22" s="66"/>
-      <c r="L22" s="38"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="35">
-        <v>98</v>
-      </c>
-      <c r="C23" s="66">
-        <v>0.73311283327999999</v>
-      </c>
-      <c r="D23" s="67">
-        <v>669.54181663717804</v>
-      </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="30">
+      <c r="C49" s="37">
+        <v>0.77900904735999899</v>
+      </c>
+      <c r="D49" s="61">
+        <v>766.16823740602399</v>
+      </c>
+      <c r="E49" s="37"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="37">
+        <v>0.77900904735999899</v>
+      </c>
+      <c r="H49" s="61">
+        <v>766.16823740602399</v>
+      </c>
+      <c r="I49" s="37"/>
+      <c r="J49" s="38"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="30">
         <v>127</v>
       </c>
-      <c r="I23" s="69">
-        <v>0.77366061472000003</v>
-      </c>
-      <c r="J23" s="70">
-        <v>766.05909267424397</v>
-      </c>
-      <c r="K23" s="69"/>
-      <c r="L23" s="26"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="30">
-        <v>99</v>
-      </c>
-      <c r="C24" s="69">
-        <v>0.73517166015999902</v>
-      </c>
-      <c r="D24" s="70">
-        <v>673.14994854116003</v>
-      </c>
-      <c r="E24" s="69"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="35">
+      <c r="C50" s="25">
+        <v>0.78056168831999895</v>
+      </c>
+      <c r="D50" s="28">
+        <v>769.58571399022799</v>
+      </c>
+      <c r="F50" s="26"/>
+      <c r="G50" s="25">
+        <v>0.78056168831999895</v>
+      </c>
+      <c r="H50" s="28">
+        <v>769.58571399022799</v>
+      </c>
+      <c r="I50" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J50" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="35">
         <v>128</v>
       </c>
-      <c r="I24" s="66">
-        <v>0.77461359967999999</v>
-      </c>
-      <c r="J24" s="67">
-        <v>769.11945411733802</v>
-      </c>
-      <c r="K24" s="66"/>
-      <c r="L24" s="38"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="35">
-        <v>100</v>
-      </c>
-      <c r="C25" s="66">
-        <v>0.73716700000000002</v>
-      </c>
-      <c r="D25" s="67">
-        <v>676.73578843719201</v>
-      </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="30">
+      <c r="C51" s="37">
+        <v>0.78211432927999902</v>
+      </c>
+      <c r="D51" s="61">
+        <v>773.00319057443198</v>
+      </c>
+      <c r="E51" s="37"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="37">
+        <v>0.78211432927999902</v>
+      </c>
+      <c r="H51" s="61">
+        <v>773.00319057443198</v>
+      </c>
+      <c r="I51" s="37"/>
+      <c r="J51" s="38"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="30">
         <v>129</v>
       </c>
-      <c r="I25" s="69">
-        <v>0.77555561775999904</v>
-      </c>
-      <c r="J25" s="70">
-        <v>772.16393611345802</v>
-      </c>
-      <c r="K25" s="69"/>
-      <c r="L25" s="26"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="30">
-        <v>101</v>
-      </c>
-      <c r="C26" s="69">
-        <v>0.73910066383999995</v>
-      </c>
-      <c r="D26" s="70">
-        <v>680.29962778714696</v>
-      </c>
-      <c r="E26" s="69"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="35">
+      <c r="C52" s="25">
+        <v>0.78366697023999898</v>
+      </c>
+      <c r="D52" s="28">
+        <v>776.42066715863598</v>
+      </c>
+      <c r="F52" s="26"/>
+      <c r="G52" s="25">
+        <v>0.78366697023999898</v>
+      </c>
+      <c r="H52" s="28">
+        <v>776.42066715863598</v>
+      </c>
+      <c r="I52" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J52" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="35">
         <v>130</v>
       </c>
-      <c r="I26" s="66">
-        <v>0.77648848000000004</v>
-      </c>
-      <c r="J26" s="67">
-        <v>775.19270258734105</v>
-      </c>
-      <c r="K26" s="66"/>
-      <c r="L26" s="38"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="35">
-        <v>102</v>
-      </c>
-      <c r="C27" s="66">
-        <v>0.74097446272</v>
-      </c>
-      <c r="D27" s="67">
-        <v>683.84175156620404</v>
-      </c>
-      <c r="E27" s="66"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="30">
+      <c r="C53" s="37">
+        <v>0.78521961119999895</v>
+      </c>
+      <c r="D53" s="61">
+        <v>779.83814374283997</v>
+      </c>
+      <c r="E53" s="37"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="37">
+        <v>0.78521961119999895</v>
+      </c>
+      <c r="H53" s="61">
+        <v>779.83814374283997</v>
+      </c>
+      <c r="I53" s="37"/>
+      <c r="J53" s="38"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="30">
         <v>131</v>
       </c>
-      <c r="I27" s="69">
-        <v>0.77741399743999995</v>
-      </c>
-      <c r="J27" s="70">
-        <v>778.20591462917196</v>
-      </c>
-      <c r="K27" s="69"/>
-      <c r="L27" s="26"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="30">
-        <v>103</v>
-      </c>
-      <c r="C28" s="69">
-        <v>0.74279020768000004</v>
-      </c>
-      <c r="D28" s="70">
-        <v>687.36243846957098</v>
-      </c>
-      <c r="E28" s="69"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="35">
+      <c r="C54" s="25">
+        <v>0.78677225215999902</v>
+      </c>
+      <c r="D54" s="28">
+        <v>783.25562032704397</v>
+      </c>
+      <c r="F54" s="26"/>
+      <c r="G54" s="25">
+        <v>0.78677225215999902</v>
+      </c>
+      <c r="H54" s="28">
+        <v>783.25562032704397</v>
+      </c>
+      <c r="I54" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J54" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="35">
         <v>132</v>
       </c>
-      <c r="I28" s="66">
-        <v>0.77833398111999996</v>
-      </c>
-      <c r="J28" s="67">
-        <v>781.20373056477001</v>
-      </c>
-      <c r="K28" s="66"/>
-      <c r="L28" s="38"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="35">
-        <v>104</v>
-      </c>
-      <c r="C29" s="66">
-        <v>0.74454970976000001</v>
-      </c>
-      <c r="D29" s="67">
-        <v>690.86196111068398</v>
-      </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="30">
+      <c r="C55" s="37">
+        <v>0.78832489311999898</v>
+      </c>
+      <c r="D55" s="61">
+        <v>786.67309691124797</v>
+      </c>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="37">
+        <v>0.78832489311999898</v>
+      </c>
+      <c r="H55" s="61">
+        <v>786.67309691124797</v>
+      </c>
+      <c r="I55" s="37"/>
+      <c r="J55" s="38"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="30">
         <v>133</v>
       </c>
-      <c r="I29" s="69">
-        <v>0.77925024208000004</v>
-      </c>
-      <c r="J29" s="70">
-        <v>784.18630602352005</v>
-      </c>
-      <c r="K29" s="69"/>
-      <c r="L29" s="26"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="30">
-        <v>105</v>
-      </c>
-      <c r="C30" s="69">
-        <v>0.74625478000000001</v>
-      </c>
-      <c r="D30" s="70">
-        <v>694.34058621127701</v>
-      </c>
-      <c r="E30" s="69"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="35">
+      <c r="C56" s="25">
+        <v>0.78987753407999906</v>
+      </c>
+      <c r="D56" s="28">
+        <v>790.09057349545196</v>
+      </c>
+      <c r="F56" s="26"/>
+      <c r="G56" s="25">
+        <v>0.78987753407999906</v>
+      </c>
+      <c r="H56" s="28">
+        <v>790.09057349545196</v>
+      </c>
+      <c r="I56" s="25">
+        <v>0.749</v>
+      </c>
+      <c r="J56" s="26">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="35">
         <v>134</v>
       </c>
-      <c r="I30" s="66">
-        <v>0.78016459135999905</v>
-      </c>
-      <c r="J30" s="67">
-        <v>787.15379400412303</v>
-      </c>
-      <c r="K30" s="66"/>
-      <c r="L30" s="38"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="35">
-        <v>106</v>
-      </c>
-      <c r="C31" s="66">
-        <v>0.74790722943999899</v>
-      </c>
-      <c r="D31" s="67">
-        <v>697.79857478373799</v>
-      </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="30">
+      <c r="C57" s="37">
+        <v>0.79143017503999902</v>
+      </c>
+      <c r="D57" s="61">
+        <v>793.50805007965596</v>
+      </c>
+      <c r="E57" s="37"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="37">
+        <v>0.79143017503999902</v>
+      </c>
+      <c r="H57" s="61">
+        <v>793.50805007965596</v>
+      </c>
+      <c r="I57" s="37"/>
+      <c r="J57" s="38"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="30">
         <v>135</v>
       </c>
-      <c r="I31" s="69">
-        <v>0.78107884000000005</v>
-      </c>
-      <c r="J31" s="70">
-        <v>790.10634493826501</v>
-      </c>
-      <c r="K31" s="69"/>
-      <c r="L31" s="26"/>
-    </row>
-    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="30">
-        <v>107</v>
-      </c>
-      <c r="C32" s="69">
-        <v>0.74950886912000003</v>
-      </c>
-      <c r="D32" s="70">
-        <v>701.23618230614795</v>
-      </c>
-      <c r="E32" s="69">
+      <c r="C58" s="25">
+        <v>0.79298281599999898</v>
+      </c>
+      <c r="D58" s="28">
+        <v>796.92552666385996</v>
+      </c>
+      <c r="F58" s="26"/>
+      <c r="G58" s="25">
+        <v>0.79298281599999898</v>
+      </c>
+      <c r="H58" s="28">
+        <v>796.92552666385996</v>
+      </c>
+      <c r="I58" s="25">
         <v>0.749</v>
       </c>
-      <c r="F32" s="26">
+      <c r="J58" s="26">
         <v>702</v>
       </c>
-      <c r="G32" s="68"/>
-      <c r="H32" s="44">
+    </row>
+    <row r="59" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="44">
         <v>136</v>
       </c>
-      <c r="I32" s="46">
-        <v>0.781336441386564</v>
-      </c>
-      <c r="J32" s="71">
-        <v>793.04410675228701</v>
-      </c>
-      <c r="K32" s="46">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="L32" s="49">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="44">
-        <v>108</v>
-      </c>
-      <c r="C33" s="46">
-        <v>0.75106151007999999</v>
-      </c>
-      <c r="D33" s="71">
-        <v>704.65365889035195</v>
-      </c>
-      <c r="E33" s="46"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
+      <c r="C59" s="46">
+        <v>0.79453545695999905</v>
+      </c>
+      <c r="D59" s="62">
+        <v>800.34300324806395</v>
+      </c>
+      <c r="E59" s="46"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="46">
+        <v>0.79453545695999905</v>
+      </c>
+      <c r="H59" s="62">
+        <v>800.34300324806395</v>
+      </c>
+      <c r="I59" s="46"/>
+      <c r="J59" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
+  <mergeCells count="8">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DB1CDE-83C4-409E-A2CA-83801EFE682C}">
+  <dimension ref="B1:J8"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="73"/>
+      <c r="C2" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="69"/>
+    </row>
+    <row r="3" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="80">
+        <v>1.1028708300000001</v>
+      </c>
+      <c r="D4" s="81">
+        <v>2.9339479700000002</v>
+      </c>
+      <c r="E4" s="82">
+        <v>2.4853261</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="74">
+        <v>1.0784661</v>
+      </c>
+      <c r="D5" s="71">
+        <v>3.40294293</v>
+      </c>
+      <c r="E5" s="75">
+        <v>2.8244687499999999</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="72">
+        <v>-1.214E-4</v>
+      </c>
+      <c r="I5" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="88" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F4:I4 F5:G5 I5" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>